<commit_message>
da sua them giangvien bang file excel
</commit_message>
<xml_diff>
--- a/file/datakhoa.xlsx
+++ b/file/datakhoa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAPTOP\Desktop\HK1-Nam4\Cong nghe moi\Do an\ProjectCongNgheMoiLayout\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioCode\data_baitaplon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45861AB2-280F-43B9-BC1D-61C0B14C0C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB9E3D1-EE41-41CF-91B2-7F33141A969E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,16 +45,16 @@
     <t>Cơ khí xăng dầu</t>
   </si>
   <si>
-    <t>CNN</t>
-  </si>
-  <si>
-    <t>CATOON</t>
-  </si>
-  <si>
-    <t>HEHE</t>
-  </si>
-  <si>
-    <t>HAHA</t>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test4</t>
   </si>
 </sst>
 </file>
@@ -382,11 +382,13 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>